<commit_message>
Added HNSM to HC list
</commit_message>
<xml_diff>
--- a/app/config/tables/OPVCOVID/Forms/OPVCOVID/OPVCOVID.xlsx
+++ b/app/config/tables/OPVCOVID/Forms/OPVCOVID/OPVCOVID.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A98749-2099-4075-925B-6820777BA2EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD9FF31-D43B-461C-BEC4-C688F4119875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="740">
   <si>
     <t>setting_name</t>
   </si>
@@ -2251,6 +2251,9 @@
   </si>
   <si>
     <t>data("HOSP5NOITE") == "1"</t>
+  </si>
+  <si>
+    <t>HNSM</t>
   </si>
 </sst>
 </file>
@@ -2787,7 +2790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787AB6FC-E5B2-448F-8A60-6571052C1548}">
   <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
@@ -9199,11 +9202,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9716,15 +9719,15 @@
       <c r="A41" t="s">
         <v>375</v>
       </c>
-      <c r="B41" s="14" t="str">
-        <f>"304"</f>
-        <v>304</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>376</v>
+      <c r="B41" s="7" t="str">
+        <f>"301"</f>
+        <v>301</v>
+      </c>
+      <c r="C41" t="s">
+        <v>739</v>
+      </c>
+      <c r="D41" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -9732,14 +9735,14 @@
         <v>375</v>
       </c>
       <c r="B42" s="14" t="str">
-        <f>"305"</f>
-        <v>305</v>
+        <f>"304"</f>
+        <v>304</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -9747,14 +9750,14 @@
         <v>375</v>
       </c>
       <c r="B43" s="14" t="str">
-        <f>"306"</f>
-        <v>306</v>
+        <f>"305"</f>
+        <v>305</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -9762,14 +9765,14 @@
         <v>375</v>
       </c>
       <c r="B44" s="14" t="str">
-        <f>"307"</f>
-        <v>307</v>
+        <f>"306"</f>
+        <v>306</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -9777,14 +9780,14 @@
         <v>375</v>
       </c>
       <c r="B45" s="14" t="str">
-        <f>"308"</f>
-        <v>308</v>
+        <f>"307"</f>
+        <v>307</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -9792,14 +9795,14 @@
         <v>375</v>
       </c>
       <c r="B46" s="14" t="str">
-        <f>"309"</f>
-        <v>309</v>
+        <f>"308"</f>
+        <v>308</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -9807,14 +9810,14 @@
         <v>375</v>
       </c>
       <c r="B47" s="14" t="str">
-        <f>"310"</f>
-        <v>310</v>
+        <f>"309"</f>
+        <v>309</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -9822,14 +9825,14 @@
         <v>375</v>
       </c>
       <c r="B48" s="14" t="str">
-        <f>"311"</f>
-        <v>311</v>
+        <f>"310"</f>
+        <v>310</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -9837,14 +9840,14 @@
         <v>375</v>
       </c>
       <c r="B49" s="14" t="str">
-        <f>"312"</f>
-        <v>312</v>
+        <f>"311"</f>
+        <v>311</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -9852,14 +9855,14 @@
         <v>375</v>
       </c>
       <c r="B50" s="14" t="str">
-        <f>"313"</f>
-        <v>313</v>
+        <f>"312"</f>
+        <v>312</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -9867,14 +9870,14 @@
         <v>375</v>
       </c>
       <c r="B51" s="14" t="str">
-        <f>"314"</f>
-        <v>314</v>
+        <f>"313"</f>
+        <v>313</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -9882,14 +9885,14 @@
         <v>375</v>
       </c>
       <c r="B52" s="14" t="str">
-        <f>"315"</f>
-        <v>315</v>
+        <f>"314"</f>
+        <v>314</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -9897,14 +9900,14 @@
         <v>375</v>
       </c>
       <c r="B53" s="14" t="str">
-        <f>"316"</f>
-        <v>316</v>
+        <f>"315"</f>
+        <v>315</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -9912,14 +9915,14 @@
         <v>375</v>
       </c>
       <c r="B54" s="14" t="str">
-        <f>"317"</f>
-        <v>317</v>
+        <f>"316"</f>
+        <v>316</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -9927,14 +9930,14 @@
         <v>375</v>
       </c>
       <c r="B55" s="14" t="str">
-        <f>"318"</f>
-        <v>318</v>
+        <f>"317"</f>
+        <v>317</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -9942,14 +9945,14 @@
         <v>375</v>
       </c>
       <c r="B56" s="14" t="str">
-        <f>"319"</f>
-        <v>319</v>
+        <f>"318"</f>
+        <v>318</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -9957,14 +9960,14 @@
         <v>375</v>
       </c>
       <c r="B57" s="14" t="str">
-        <f>"320"</f>
-        <v>320</v>
+        <f>"319"</f>
+        <v>319</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -9972,14 +9975,14 @@
         <v>375</v>
       </c>
       <c r="B58" s="14" t="str">
-        <f>"321"</f>
-        <v>321</v>
+        <f>"320"</f>
+        <v>320</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -9987,14 +9990,14 @@
         <v>375</v>
       </c>
       <c r="B59" s="14" t="str">
-        <f>"322"</f>
-        <v>322</v>
+        <f>"321"</f>
+        <v>321</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -10002,14 +10005,14 @@
         <v>375</v>
       </c>
       <c r="B60" s="14" t="str">
-        <f>"323"</f>
-        <v>323</v>
+        <f>"322"</f>
+        <v>322</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -10017,14 +10020,14 @@
         <v>375</v>
       </c>
       <c r="B61" s="14" t="str">
-        <f>"324"</f>
-        <v>324</v>
+        <f>"323"</f>
+        <v>323</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -10032,18 +10035,30 @@
         <v>375</v>
       </c>
       <c r="B62" s="14" t="str">
+        <f>"324"</f>
+        <v>324</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>375</v>
+      </c>
+      <c r="B63" s="14" t="str">
         <f>"325"</f>
         <v>325</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>397</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D63" s="14" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
@@ -10059,7 +10074,6 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="7"/>
@@ -10086,10 +10100,10 @@
       <c r="C74" s="7"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="7"/>
       <c r="C75" s="7"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="7"/>
       <c r="C76" s="7"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
@@ -10162,6 +10176,7 @@
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="7"/>
@@ -10181,8 +10196,8 @@
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="7"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="7"/>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="7"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="7"/>
@@ -10234,6 +10249,9 @@
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="7"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Adding Sona as assistant
</commit_message>
<xml_diff>
--- a/app/config/tables/OPVCOVID/Forms/OPVCOVID/OPVCOVID.xlsx
+++ b/app/config/tables/OPVCOVID/Forms/OPVCOVID/OPVCOVID.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D092A90-C90C-4B9B-A049-43287918E3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710ED8D3-8F4B-4D3C-BBFF-0D27B9A30C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2392" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="744">
   <si>
     <t>setting_name</t>
   </si>
@@ -2263,6 +2263,9 @@
   </si>
   <si>
     <t>Idrissa</t>
+  </si>
+  <si>
+    <t>Sona</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2368,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2388,7 +2391,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2800,9 +2802,9 @@
   <dimension ref="A1:O110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9211,11 +9213,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9240,7 +9242,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>707</v>
       </c>
@@ -9255,7 +9257,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>707</v>
       </c>
@@ -9270,7 +9272,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>707</v>
       </c>
@@ -9285,7 +9287,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>707</v>
       </c>
@@ -9300,7 +9302,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>707</v>
       </c>
@@ -9315,7 +9317,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>707</v>
       </c>
@@ -9330,40 +9332,40 @@
         <v>742</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>554</v>
-      </c>
-      <c r="B9" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>632</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>630</v>
-      </c>
+    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>707</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"7"</f>
+        <v>7</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>554</v>
       </c>
       <c r="B10" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -9371,96 +9373,96 @@
         <v>554</v>
       </c>
       <c r="B11" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>555</v>
+        <v>633</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>556</v>
+        <v>631</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>554</v>
       </c>
-      <c r="B12" s="13" t="str">
+      <c r="B12" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>555</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>554</v>
+      </c>
+      <c r="B13" s="13" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>634</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-    </row>
     <row r="14" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>63</v>
       </c>
       <c r="B15" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="D17" t="s">
-        <v>698</v>
-      </c>
-    </row>
+    <row r="17" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>70</v>
       </c>
       <c r="B18" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>562</v>
+        <v>699</v>
+      </c>
+      <c r="D18" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -9468,65 +9470,65 @@
         <v>70</v>
       </c>
       <c r="B19" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="13" t="str">
+      <c r="B20" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="13" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D21" s="13" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
     <row r="22" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
-        <v>683</v>
-      </c>
-      <c r="B22" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>684</v>
-      </c>
-      <c r="D22" t="s">
-        <v>685</v>
-      </c>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>683</v>
       </c>
       <c r="B23" t="str">
-        <f>"4"</f>
-        <v>4</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D23" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -9534,14 +9536,14 @@
         <v>683</v>
       </c>
       <c r="B24" t="str">
-        <f>"5"</f>
-        <v>5</v>
+        <f>"4"</f>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D24" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -9549,14 +9551,14 @@
         <v>683</v>
       </c>
       <c r="B25" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"5"</f>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>703</v>
+        <v>688</v>
       </c>
       <c r="D25" t="s">
-        <v>704</v>
+        <v>689</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
@@ -9564,50 +9566,50 @@
         <v>683</v>
       </c>
       <c r="B26" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>703</v>
+      </c>
+      <c r="D26" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="B27" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>690</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>42</v>
-      </c>
+    <row r="28" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
       <c r="B29" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -9615,47 +9617,47 @@
         <v>69</v>
       </c>
       <c r="B30" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>41</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B32" t="str">
+      <c r="B33" t="str">
         <f>"D:NS,M:NS,Y:NS"</f>
         <v>D:NS,M:NS,Y:NS</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>50</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>332</v>
-      </c>
-      <c r="B34" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>334</v>
-      </c>
-      <c r="D34" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -9663,14 +9665,14 @@
         <v>332</v>
       </c>
       <c r="B35" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D35" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -9678,47 +9680,47 @@
         <v>332</v>
       </c>
       <c r="B36" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>335</v>
+      </c>
+      <c r="D36" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>332</v>
+      </c>
+      <c r="B37" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>336</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="7"/>
-    </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>397</v>
-      </c>
-      <c r="B38" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C38" s="15">
-        <v>1</v>
-      </c>
-      <c r="D38" s="15">
-        <v>1</v>
-      </c>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>397</v>
       </c>
       <c r="B39" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="C39" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -9726,77 +9728,77 @@
         <v>397</v>
       </c>
       <c r="B40" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C40" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>397</v>
       </c>
-      <c r="B41" s="13" t="str">
-        <f>"4"</f>
-        <v>4</v>
+      <c r="B41" t="str">
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C41" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>397</v>
       </c>
-      <c r="B42" s="7" t="str">
+      <c r="B42" s="13" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C42" s="15">
+        <v>4</v>
+      </c>
+      <c r="D42" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>397</v>
+      </c>
+      <c r="B43" s="7" t="str">
         <f>"5"</f>
         <v>5</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>399</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="7"/>
-    </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>375</v>
-      </c>
-      <c r="B44" s="7" t="str">
-        <f>"301"</f>
-        <v>301</v>
-      </c>
-      <c r="C44" t="s">
-        <v>735</v>
-      </c>
-      <c r="D44" t="s">
-        <v>735</v>
-      </c>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>375</v>
       </c>
-      <c r="B45" s="14" t="str">
-        <f>"304"</f>
-        <v>304</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>376</v>
+      <c r="B45" s="7" t="str">
+        <f>"301"</f>
+        <v>301</v>
+      </c>
+      <c r="C45" t="s">
+        <v>735</v>
+      </c>
+      <c r="D45" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -9804,14 +9806,14 @@
         <v>375</v>
       </c>
       <c r="B46" s="14" t="str">
-        <f>"305"</f>
-        <v>305</v>
+        <f>"304"</f>
+        <v>304</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -9819,14 +9821,14 @@
         <v>375</v>
       </c>
       <c r="B47" s="14" t="str">
-        <f>"306"</f>
-        <v>306</v>
+        <f>"305"</f>
+        <v>305</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -9834,14 +9836,14 @@
         <v>375</v>
       </c>
       <c r="B48" s="14" t="str">
-        <f>"307"</f>
-        <v>307</v>
+        <f>"306"</f>
+        <v>306</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -9849,14 +9851,14 @@
         <v>375</v>
       </c>
       <c r="B49" s="14" t="str">
-        <f>"308"</f>
-        <v>308</v>
+        <f>"307"</f>
+        <v>307</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -9864,14 +9866,14 @@
         <v>375</v>
       </c>
       <c r="B50" s="14" t="str">
-        <f>"309"</f>
-        <v>309</v>
+        <f>"308"</f>
+        <v>308</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -9879,14 +9881,14 @@
         <v>375</v>
       </c>
       <c r="B51" s="14" t="str">
-        <f>"310"</f>
-        <v>310</v>
+        <f>"309"</f>
+        <v>309</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>737</v>
+        <v>381</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>737</v>
+        <v>381</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -9894,14 +9896,14 @@
         <v>375</v>
       </c>
       <c r="B52" s="14" t="str">
-        <f>"311"</f>
-        <v>311</v>
+        <f>"310"</f>
+        <v>310</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>382</v>
+        <v>737</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>382</v>
+        <v>737</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -9909,14 +9911,14 @@
         <v>375</v>
       </c>
       <c r="B53" s="14" t="str">
-        <f>"312"</f>
-        <v>312</v>
+        <f>"311"</f>
+        <v>311</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -9924,14 +9926,14 @@
         <v>375</v>
       </c>
       <c r="B54" s="14" t="str">
-        <f>"313"</f>
-        <v>313</v>
+        <f>"312"</f>
+        <v>312</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -9939,14 +9941,14 @@
         <v>375</v>
       </c>
       <c r="B55" s="14" t="str">
-        <f>"314"</f>
-        <v>314</v>
+        <f>"313"</f>
+        <v>313</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -9954,14 +9956,14 @@
         <v>375</v>
       </c>
       <c r="B56" s="14" t="str">
-        <f>"315"</f>
-        <v>315</v>
+        <f>"314"</f>
+        <v>314</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -9969,14 +9971,14 @@
         <v>375</v>
       </c>
       <c r="B57" s="14" t="str">
-        <f>"316"</f>
-        <v>316</v>
+        <f>"315"</f>
+        <v>315</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -9984,14 +9986,14 @@
         <v>375</v>
       </c>
       <c r="B58" s="14" t="str">
-        <f>"317"</f>
-        <v>317</v>
+        <f>"316"</f>
+        <v>316</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -9999,14 +10001,14 @@
         <v>375</v>
       </c>
       <c r="B59" s="14" t="str">
-        <f>"318"</f>
-        <v>318</v>
+        <f>"317"</f>
+        <v>317</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -10014,14 +10016,14 @@
         <v>375</v>
       </c>
       <c r="B60" s="14" t="str">
-        <f>"319"</f>
-        <v>319</v>
+        <f>"318"</f>
+        <v>318</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -10029,14 +10031,14 @@
         <v>375</v>
       </c>
       <c r="B61" s="14" t="str">
-        <f>"320"</f>
-        <v>320</v>
+        <f>"319"</f>
+        <v>319</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -10044,14 +10046,14 @@
         <v>375</v>
       </c>
       <c r="B62" s="14" t="str">
-        <f>"321"</f>
-        <v>321</v>
+        <f>"320"</f>
+        <v>320</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -10059,14 +10061,14 @@
         <v>375</v>
       </c>
       <c r="B63" s="14" t="str">
-        <f>"322"</f>
-        <v>322</v>
+        <f>"321"</f>
+        <v>321</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -10074,14 +10076,14 @@
         <v>375</v>
       </c>
       <c r="B64" s="14" t="str">
-        <f>"323"</f>
-        <v>323</v>
+        <f>"322"</f>
+        <v>322</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -10089,14 +10091,14 @@
         <v>375</v>
       </c>
       <c r="B65" s="14" t="str">
-        <f>"324"</f>
-        <v>324</v>
+        <f>"323"</f>
+        <v>323</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -10104,18 +10106,30 @@
         <v>375</v>
       </c>
       <c r="B66" s="14" t="str">
+        <f>"324"</f>
+        <v>324</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>375</v>
+      </c>
+      <c r="B67" s="14" t="str">
         <f>"325"</f>
         <v>325</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C67" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D67" s="14" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B67" s="7"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B68" s="7"/>
@@ -10131,7 +10145,6 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B73" s="7"/>
@@ -10158,10 +10171,10 @@
       <c r="C78" s="7"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B79" s="7"/>
       <c r="C79" s="7"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B80" s="7"/>
       <c r="C80" s="7"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
@@ -10234,6 +10247,7 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99" s="7"/>
@@ -10253,8 +10267,8 @@
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104" s="7"/>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B106" s="7"/>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B105" s="7"/>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107" s="7"/>
@@ -10306,6 +10320,9 @@
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B123" s="7"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B124" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -10712,7 +10729,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="18"/>
+      <c r="A22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">

</xml_diff>

<commit_message>
choicelist for symptoms amended, getresults interview constraints changed
</commit_message>
<xml_diff>
--- a/app/config/tables/OPVCOVID/Forms/OPVCOVID/OPVCOVID.xlsx
+++ b/app/config/tables/OPVCOVID/Forms/OPVCOVID/OPVCOVID.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C02C8-DA29-49F0-BF7F-E6C33760FF9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29082F3D-D82C-46ED-A1CB-7125A1AD6EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -2274,51 +2274,6 @@
     <t>data("ASSISTENTE") != null</t>
   </si>
   <si>
-    <t>data("CONSTI") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("TOSSE") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("FEBRE") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("DISPNE") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("VOMITO") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("DIARRE") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("OLFATO") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("PALADA") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("CABECA") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("GARGAN") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("CORPO") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("CONSAC") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("OUSIN1") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("PESO") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
-    <t>data("CONS") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
     <t>data("CONSNUM") != null || data("CONS") != '1'</t>
   </si>
   <si>
@@ -2337,9 +2292,6 @@
     <t>data("CONS5DATA") != null || data("CONS") != '1' || data('CONSNUM')=='1' || data('CONSNUM')=='2' || data('CONSNUM')=='3' || data('CONSNUM')=='4'</t>
   </si>
   <si>
-    <t>data("HOSP") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
     <t>data("HOSPNUM") != null || data("HOSP") != '1'</t>
   </si>
   <si>
@@ -2355,9 +2307,6 @@
     <t>data("HOSP4DATA") != null || data("HOSP") != '1' || data("HOSPNUM") == '1' || data("HOSPNUM") == '2' || data("HOSPNUM") == '3'</t>
   </si>
   <si>
-    <t>data("MEDICA") != null || data("ESTADO") == null</t>
-  </si>
-  <si>
     <t>data("COVID") != null || data("ESTADO") == null</t>
   </si>
   <si>
@@ -2514,12 +2463,6 @@
     <t>data("HOSP5ONDE") != null || data("HOSP5DATA") == null</t>
   </si>
   <si>
-    <t xml:space="preserve">data("MEDICAQU") != null || data("ESTADO") == null || data("MEDICA") == '2' </t>
-  </si>
-  <si>
-    <t>data("OUSIN2") != null ||data("OUSIN1") == '2' || data("OUSIN1") == '3'|| data("ESTADO") == null</t>
-  </si>
-  <si>
     <t>data("INF")!= null || data("ESTADO") == null</t>
   </si>
   <si>
@@ -2536,6 +2479,63 @@
   </si>
   <si>
     <t>data("HOSP5NODIA") != null  || data("HOSP5NOITE")=='3'|| data("HOSP5NOITE")=='2'|| data("HOSP5DATA") == null</t>
+  </si>
+  <si>
+    <t>data("CONSTI") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("TOSSE") != null || data("ESTADO") == null|| data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("FEBRE") != null || data("ESTADO") == null|| data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("DISPNE") != null || data("ESTADO") == null|| data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("VOMITO") != null || data("ESTADO") == null|| data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("DIARRE") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("OLFATO") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("PALADA") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("CABECA") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("GARGAN") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("CORPO") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("CONSAC") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("OUSIN1") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("OUSIN2") != null ||data("OUSIN1") == '2' || data("OUSIN1") == '3'|| data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("PESO") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("CONS") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("HOSP") != null || data("ESTADO") == null || data("GETRESULTS")=='1'</t>
+  </si>
+  <si>
+    <t>data("MEDICA") != null || data("ESTADO") == null || data("GETRESULTS") == '1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data("MEDICAQU") != null || data("ESTADO") == null || data("MEDICA") != '1' </t>
   </si>
 </sst>
 </file>
@@ -3608,7 +3608,7 @@
         <v>629</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>828</v>
+        <v>809</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
@@ -3636,7 +3636,7 @@
         <v>604</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>785</v>
+        <v>768</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -3901,7 +3901,7 @@
         <v>697</v>
       </c>
       <c r="J73" s="18" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
@@ -3951,7 +3951,7 @@
         <v>695</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
@@ -3989,9 +3989,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E034F7AB-A88F-4084-9C1D-FD9CFEAF70F4}">
   <dimension ref="A1:O484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J458" sqref="J458"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A448" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J460" sqref="J460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4114,7 +4114,7 @@
         <v>84</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>746</v>
+        <v>815</v>
       </c>
       <c r="K7" t="s">
         <v>83</v>
@@ -4288,7 +4288,7 @@
         <v>115</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>747</v>
+        <v>816</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -4457,7 +4457,7 @@
         <v>130</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>748</v>
+        <v>817</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -4626,7 +4626,7 @@
         <v>134</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>749</v>
+        <v>818</v>
       </c>
       <c r="K43" t="s">
         <v>150</v>
@@ -4801,7 +4801,7 @@
         <v>165</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>750</v>
+        <v>819</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -4970,7 +4970,7 @@
         <v>179</v>
       </c>
       <c r="J67" s="19" t="s">
-        <v>751</v>
+        <v>820</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
@@ -5139,7 +5139,7 @@
         <v>194</v>
       </c>
       <c r="J79" s="19" t="s">
-        <v>752</v>
+        <v>821</v>
       </c>
       <c r="K79" t="s">
         <v>225</v>
@@ -5314,7 +5314,7 @@
         <v>210</v>
       </c>
       <c r="J91" s="19" t="s">
-        <v>753</v>
+        <v>822</v>
       </c>
       <c r="K91" t="s">
         <v>227</v>
@@ -5489,7 +5489,7 @@
         <v>229</v>
       </c>
       <c r="J103" s="19" t="s">
-        <v>754</v>
+        <v>823</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
@@ -5658,7 +5658,7 @@
         <v>244</v>
       </c>
       <c r="J115" s="19" t="s">
-        <v>755</v>
+        <v>824</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
@@ -5827,7 +5827,7 @@
         <v>258</v>
       </c>
       <c r="J127" s="19" t="s">
-        <v>756</v>
+        <v>825</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
@@ -5996,7 +5996,7 @@
         <v>702</v>
       </c>
       <c r="J139" s="19" t="s">
-        <v>757</v>
+        <v>826</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
@@ -6165,7 +6165,7 @@
         <v>275</v>
       </c>
       <c r="J151" s="19" t="s">
-        <v>758</v>
+        <v>827</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.35">
@@ -6359,7 +6359,7 @@
         <v>307</v>
       </c>
       <c r="J165" s="19" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.35">
@@ -6549,7 +6549,7 @@
         <v>310</v>
       </c>
       <c r="J179" s="19" t="s">
-        <v>759</v>
+        <v>829</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.35">
@@ -6594,7 +6594,7 @@
         <v>352</v>
       </c>
       <c r="J183" s="19" t="s">
-        <v>760</v>
+        <v>830</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.35">
@@ -6622,7 +6622,7 @@
         <v>411</v>
       </c>
       <c r="J185" s="19" t="s">
-        <v>761</v>
+        <v>746</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.35">
@@ -6688,7 +6688,7 @@
         <v>341</v>
       </c>
       <c r="J192" s="19" t="s">
-        <v>762</v>
+        <v>747</v>
       </c>
     </row>
     <row r="193" spans="2:10" x14ac:dyDescent="0.35">
@@ -6754,7 +6754,7 @@
         <v>346</v>
       </c>
       <c r="J198" s="21" t="s">
-        <v>802</v>
+        <v>785</v>
       </c>
     </row>
     <row r="199" spans="2:10" x14ac:dyDescent="0.35">
@@ -6774,7 +6774,7 @@
         <v>347</v>
       </c>
       <c r="J199" s="21" t="s">
-        <v>803</v>
+        <v>786</v>
       </c>
     </row>
     <row r="200" spans="2:10" x14ac:dyDescent="0.35">
@@ -6799,7 +6799,7 @@
         <v>350</v>
       </c>
       <c r="J201" s="21" t="s">
-        <v>805</v>
+        <v>788</v>
       </c>
     </row>
     <row r="202" spans="2:10" x14ac:dyDescent="0.35">
@@ -6856,7 +6856,7 @@
         <v>344</v>
       </c>
       <c r="J207" s="21" t="s">
-        <v>804</v>
+        <v>787</v>
       </c>
     </row>
     <row r="208" spans="2:10" x14ac:dyDescent="0.35">
@@ -6921,7 +6921,7 @@
         <v>341</v>
       </c>
       <c r="J214" s="19" t="s">
-        <v>763</v>
+        <v>748</v>
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.35">
@@ -6987,7 +6987,7 @@
         <v>346</v>
       </c>
       <c r="J220" s="21" t="s">
-        <v>806</v>
+        <v>789</v>
       </c>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.35">
@@ -7007,7 +7007,7 @@
         <v>347</v>
       </c>
       <c r="J221" s="21" t="s">
-        <v>807</v>
+        <v>790</v>
       </c>
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.35">
@@ -7032,7 +7032,7 @@
         <v>350</v>
       </c>
       <c r="J223" s="21" t="s">
-        <v>808</v>
+        <v>791</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.35">
@@ -7089,7 +7089,7 @@
         <v>344</v>
       </c>
       <c r="J229" s="21" t="s">
-        <v>809</v>
+        <v>792</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.35">
@@ -7154,7 +7154,7 @@
         <v>341</v>
       </c>
       <c r="J236" s="19" t="s">
-        <v>764</v>
+        <v>749</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.35">
@@ -7220,7 +7220,7 @@
         <v>346</v>
       </c>
       <c r="J242" s="21" t="s">
-        <v>810</v>
+        <v>793</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.35">
@@ -7240,7 +7240,7 @@
         <v>347</v>
       </c>
       <c r="J243" s="21" t="s">
-        <v>811</v>
+        <v>794</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.35">
@@ -7265,7 +7265,7 @@
         <v>350</v>
       </c>
       <c r="J245" s="21" t="s">
-        <v>812</v>
+        <v>795</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.35">
@@ -7322,7 +7322,7 @@
         <v>344</v>
       </c>
       <c r="J251" s="21" t="s">
-        <v>813</v>
+        <v>796</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.35">
@@ -7387,7 +7387,7 @@
         <v>341</v>
       </c>
       <c r="J258" s="19" t="s">
-        <v>765</v>
+        <v>750</v>
       </c>
     </row>
     <row r="259" spans="2:10" x14ac:dyDescent="0.35">
@@ -7453,7 +7453,7 @@
         <v>346</v>
       </c>
       <c r="J264" s="21" t="s">
-        <v>814</v>
+        <v>797</v>
       </c>
     </row>
     <row r="265" spans="2:10" x14ac:dyDescent="0.35">
@@ -7473,7 +7473,7 @@
         <v>347</v>
       </c>
       <c r="J265" s="21" t="s">
-        <v>815</v>
+        <v>798</v>
       </c>
     </row>
     <row r="266" spans="2:10" x14ac:dyDescent="0.35">
@@ -7498,7 +7498,7 @@
         <v>350</v>
       </c>
       <c r="J267" s="21" t="s">
-        <v>816</v>
+        <v>799</v>
       </c>
     </row>
     <row r="268" spans="2:10" x14ac:dyDescent="0.35">
@@ -7555,7 +7555,7 @@
         <v>344</v>
       </c>
       <c r="J273" s="21" t="s">
-        <v>817</v>
+        <v>800</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.35">
@@ -7620,7 +7620,7 @@
         <v>341</v>
       </c>
       <c r="J280" s="19" t="s">
-        <v>766</v>
+        <v>751</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.35">
@@ -7686,7 +7686,7 @@
         <v>346</v>
       </c>
       <c r="J286" s="21" t="s">
-        <v>818</v>
+        <v>801</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.35">
@@ -7706,7 +7706,7 @@
         <v>347</v>
       </c>
       <c r="J287" s="21" t="s">
-        <v>819</v>
+        <v>802</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.35">
@@ -7731,7 +7731,7 @@
         <v>350</v>
       </c>
       <c r="J289" s="21" t="s">
-        <v>820</v>
+        <v>803</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.35">
@@ -7788,7 +7788,7 @@
         <v>344</v>
       </c>
       <c r="J295" s="21" t="s">
-        <v>821</v>
+        <v>804</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.35">
@@ -7837,7 +7837,7 @@
         <v>353</v>
       </c>
       <c r="J300" s="19" t="s">
-        <v>767</v>
+        <v>831</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.35">
@@ -7865,7 +7865,7 @@
         <v>474</v>
       </c>
       <c r="J302" s="19" t="s">
-        <v>768</v>
+        <v>752</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.35">
@@ -7930,7 +7930,7 @@
         <v>355</v>
       </c>
       <c r="J309" s="19" t="s">
-        <v>769</v>
+        <v>753</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.35">
@@ -7999,7 +7999,7 @@
         <v>717</v>
       </c>
       <c r="J315" s="21" t="s">
-        <v>786</v>
+        <v>769</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.35">
@@ -8024,7 +8024,7 @@
         <v>719</v>
       </c>
       <c r="J317" s="21" t="s">
-        <v>829</v>
+        <v>810</v>
       </c>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.35">
@@ -8078,7 +8078,7 @@
         <v>356</v>
       </c>
       <c r="J323" s="21" t="s">
-        <v>787</v>
+        <v>770</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.35">
@@ -8098,7 +8098,7 @@
         <v>347</v>
       </c>
       <c r="J324" s="21" t="s">
-        <v>788</v>
+        <v>771</v>
       </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.35">
@@ -8123,7 +8123,7 @@
         <v>350</v>
       </c>
       <c r="J326" s="21" t="s">
-        <v>779</v>
+        <v>762</v>
       </c>
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.35">
@@ -8180,7 +8180,7 @@
         <v>344</v>
       </c>
       <c r="J332" s="21" t="s">
-        <v>789</v>
+        <v>772</v>
       </c>
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.35">
@@ -8245,7 +8245,7 @@
         <v>355</v>
       </c>
       <c r="J339" s="19" t="s">
-        <v>770</v>
+        <v>754</v>
       </c>
     </row>
     <row r="340" spans="2:10" x14ac:dyDescent="0.35">
@@ -8315,7 +8315,7 @@
         <v>717</v>
       </c>
       <c r="J345" s="21" t="s">
-        <v>790</v>
+        <v>773</v>
       </c>
     </row>
     <row r="346" spans="2:10" x14ac:dyDescent="0.35">
@@ -8340,7 +8340,7 @@
         <v>719</v>
       </c>
       <c r="J347" s="21" t="s">
-        <v>830</v>
+        <v>811</v>
       </c>
     </row>
     <row r="348" spans="2:10" x14ac:dyDescent="0.35">
@@ -8394,7 +8394,7 @@
         <v>356</v>
       </c>
       <c r="J353" s="21" t="s">
-        <v>791</v>
+        <v>774</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.35">
@@ -8414,7 +8414,7 @@
         <v>347</v>
       </c>
       <c r="J354" s="21" t="s">
-        <v>792</v>
+        <v>775</v>
       </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.35">
@@ -8439,7 +8439,7 @@
         <v>350</v>
       </c>
       <c r="J356" s="21" t="s">
-        <v>780</v>
+        <v>763</v>
       </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.35">
@@ -8496,7 +8496,7 @@
         <v>344</v>
       </c>
       <c r="J362" s="21" t="s">
-        <v>822</v>
+        <v>805</v>
       </c>
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.35">
@@ -8561,7 +8561,7 @@
         <v>355</v>
       </c>
       <c r="J369" s="19" t="s">
-        <v>771</v>
+        <v>755</v>
       </c>
     </row>
     <row r="370" spans="2:10" x14ac:dyDescent="0.35">
@@ -8630,7 +8630,7 @@
         <v>717</v>
       </c>
       <c r="J375" s="21" t="s">
-        <v>793</v>
+        <v>776</v>
       </c>
     </row>
     <row r="376" spans="2:10" x14ac:dyDescent="0.35">
@@ -8655,7 +8655,7 @@
         <v>719</v>
       </c>
       <c r="J377" s="21" t="s">
-        <v>831</v>
+        <v>812</v>
       </c>
     </row>
     <row r="378" spans="2:10" x14ac:dyDescent="0.35">
@@ -8709,7 +8709,7 @@
         <v>356</v>
       </c>
       <c r="J383" s="21" t="s">
-        <v>794</v>
+        <v>777</v>
       </c>
     </row>
     <row r="384" spans="2:10" x14ac:dyDescent="0.35">
@@ -8729,7 +8729,7 @@
         <v>347</v>
       </c>
       <c r="J384" s="21" t="s">
-        <v>795</v>
+        <v>778</v>
       </c>
     </row>
     <row r="385" spans="1:10" x14ac:dyDescent="0.35">
@@ -8754,7 +8754,7 @@
         <v>350</v>
       </c>
       <c r="J386" s="21" t="s">
-        <v>781</v>
+        <v>764</v>
       </c>
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.35">
@@ -8811,7 +8811,7 @@
         <v>344</v>
       </c>
       <c r="J392" s="21" t="s">
-        <v>823</v>
+        <v>806</v>
       </c>
     </row>
     <row r="393" spans="1:10" x14ac:dyDescent="0.35">
@@ -8876,7 +8876,7 @@
         <v>355</v>
       </c>
       <c r="J399" s="19" t="s">
-        <v>772</v>
+        <v>756</v>
       </c>
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.35">
@@ -8945,7 +8945,7 @@
         <v>717</v>
       </c>
       <c r="J405" s="21" t="s">
-        <v>796</v>
+        <v>779</v>
       </c>
     </row>
     <row r="406" spans="2:10" x14ac:dyDescent="0.35">
@@ -8970,7 +8970,7 @@
         <v>719</v>
       </c>
       <c r="J407" s="21" t="s">
-        <v>832</v>
+        <v>813</v>
       </c>
     </row>
     <row r="408" spans="2:10" x14ac:dyDescent="0.35">
@@ -9024,7 +9024,7 @@
         <v>356</v>
       </c>
       <c r="J413" s="21" t="s">
-        <v>797</v>
+        <v>780</v>
       </c>
     </row>
     <row r="414" spans="2:10" x14ac:dyDescent="0.35">
@@ -9044,7 +9044,7 @@
         <v>347</v>
       </c>
       <c r="J414" s="21" t="s">
-        <v>798</v>
+        <v>781</v>
       </c>
     </row>
     <row r="415" spans="2:10" x14ac:dyDescent="0.35">
@@ -9069,7 +9069,7 @@
         <v>350</v>
       </c>
       <c r="J416" s="21" t="s">
-        <v>782</v>
+        <v>765</v>
       </c>
     </row>
     <row r="417" spans="1:10" x14ac:dyDescent="0.35">
@@ -9126,7 +9126,7 @@
         <v>344</v>
       </c>
       <c r="J422" s="21" t="s">
-        <v>824</v>
+        <v>807</v>
       </c>
     </row>
     <row r="423" spans="1:10" x14ac:dyDescent="0.35">
@@ -9191,7 +9191,7 @@
         <v>355</v>
       </c>
       <c r="J429" s="19" t="s">
-        <v>783</v>
+        <v>766</v>
       </c>
     </row>
     <row r="430" spans="1:10" x14ac:dyDescent="0.35">
@@ -9260,7 +9260,7 @@
         <v>717</v>
       </c>
       <c r="J435" s="21" t="s">
-        <v>799</v>
+        <v>782</v>
       </c>
     </row>
     <row r="436" spans="2:10" x14ac:dyDescent="0.35">
@@ -9285,7 +9285,7 @@
         <v>719</v>
       </c>
       <c r="J437" s="21" t="s">
-        <v>833</v>
+        <v>814</v>
       </c>
     </row>
     <row r="438" spans="2:10" x14ac:dyDescent="0.35">
@@ -9339,7 +9339,7 @@
         <v>356</v>
       </c>
       <c r="J443" s="21" t="s">
-        <v>800</v>
+        <v>783</v>
       </c>
     </row>
     <row r="444" spans="2:10" x14ac:dyDescent="0.35">
@@ -9359,7 +9359,7 @@
         <v>347</v>
       </c>
       <c r="J444" s="21" t="s">
-        <v>801</v>
+        <v>784</v>
       </c>
     </row>
     <row r="445" spans="2:10" x14ac:dyDescent="0.35">
@@ -9384,7 +9384,7 @@
         <v>350</v>
       </c>
       <c r="J446" s="21" t="s">
-        <v>784</v>
+        <v>767</v>
       </c>
     </row>
     <row r="447" spans="2:10" x14ac:dyDescent="0.35">
@@ -9441,7 +9441,7 @@
         <v>344</v>
       </c>
       <c r="J452" s="21" t="s">
-        <v>825</v>
+        <v>808</v>
       </c>
     </row>
     <row r="453" spans="1:10" x14ac:dyDescent="0.35">
@@ -9490,7 +9490,7 @@
         <v>359</v>
       </c>
       <c r="J457" s="19" t="s">
-        <v>773</v>
+        <v>832</v>
       </c>
     </row>
     <row r="458" spans="1:10" x14ac:dyDescent="0.35">
@@ -9515,7 +9515,7 @@
         <v>362</v>
       </c>
       <c r="J459" s="22" t="s">
-        <v>826</v>
+        <v>833</v>
       </c>
     </row>
     <row r="460" spans="1:10" x14ac:dyDescent="0.35">
@@ -9564,7 +9564,7 @@
         <v>364</v>
       </c>
       <c r="J464" s="19" t="s">
-        <v>774</v>
+        <v>757</v>
       </c>
     </row>
     <row r="465" spans="1:15" x14ac:dyDescent="0.35">
@@ -9584,7 +9584,7 @@
         <v>365</v>
       </c>
       <c r="J465" s="19" t="s">
-        <v>775</v>
+        <v>758</v>
       </c>
     </row>
     <row r="466" spans="1:15" x14ac:dyDescent="0.35">
@@ -9612,7 +9612,7 @@
         <v>368</v>
       </c>
       <c r="J467" s="19" t="s">
-        <v>776</v>
+        <v>759</v>
       </c>
     </row>
     <row r="468" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>